<commit_message>
Initial changes for fan designed promo packs
</commit_message>
<xml_diff>
--- a/i18n/template.xlsx
+++ b/i18n/template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="1021">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -3068,6 +3068,24 @@
   </si>
   <si>
     <t xml:space="preserve">of cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Asian Avians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds of Canada / Oiseaux du Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds of Continental Europe / Ngā Manu o Aotearoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds of New Zealand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds of U.S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">British Birds</t>
   </si>
   <si>
     <t xml:space="preserve">Value</t>
@@ -3097,19 +3115,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="12"/>
@@ -3489,7 +3504,7 @@
       <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.88"/>
@@ -10189,9 +10204,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -10199,7 +10214,7 @@
       <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.67"/>
@@ -10533,11 +10548,6 @@
       <c r="C28" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="0"/>
-      <c r="E28" s="0"/>
-      <c r="F28" s="0"/>
-      <c r="G28" s="0"/>
-      <c r="H28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -10549,11 +10559,6 @@
       <c r="C29" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="0"/>
-      <c r="E29" s="0"/>
-      <c r="F29" s="0"/>
-      <c r="G29" s="0"/>
-      <c r="H29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
@@ -10565,11 +10570,6 @@
       <c r="C30" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="0"/>
-      <c r="E30" s="0"/>
-      <c r="F30" s="0"/>
-      <c r="G30" s="0"/>
-      <c r="H30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
@@ -10581,11 +10581,6 @@
       <c r="C31" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="0"/>
-      <c r="E31" s="0"/>
-      <c r="F31" s="0"/>
-      <c r="G31" s="0"/>
-      <c r="H31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
@@ -10597,11 +10592,6 @@
       <c r="C32" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="0"/>
-      <c r="E32" s="0"/>
-      <c r="F32" s="0"/>
-      <c r="G32" s="0"/>
-      <c r="H32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
@@ -10887,31 +10877,6 @@
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0"/>
-      <c r="B54" s="0"/>
-      <c r="C54" s="0"/>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0"/>
-      <c r="B55" s="0"/>
-      <c r="C55" s="0"/>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0"/>
-      <c r="B56" s="0"/>
-      <c r="C56" s="0"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0"/>
-      <c r="B57" s="0"/>
-      <c r="C57" s="0"/>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0"/>
-      <c r="B58" s="0"/>
-      <c r="C58" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -10935,16 +10900,16 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="49.7"/>
@@ -11622,8 +11587,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;KffffffStrona &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffStrona &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -11634,15 +11599,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.56"/>
@@ -11656,35 +11621,81 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>1007</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>1008</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>1009</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>1010</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>1011</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>1012</v>
       </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -11713,7 +11724,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.95"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="11.53"/>
@@ -11724,12 +11735,12 @@
         <v>908</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>1013</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>1014</v>
+      <c r="A2" s="2" t="s">
+        <v>1020</v>
       </c>
     </row>
   </sheetData>
@@ -11738,8 +11749,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;KffffffStrona &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffStrona &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Initial changes for fan designed promo packs (#92)
* Initial changes for fan designed promo packs

* Initial changes for fan designed promo packs

minor clean up

* Add all cards from Travis, and update SVGs

* Follow up changes for fan designed promo packs

* Remove Swift Start filter, update bonus card icon

* Fix yellow-billed magpie

* Reindex promo cards and add silhouettes

---------

Co-authored-by: Matej Cief <matej.cief@gmail.com>
</commit_message>
<xml_diff>
--- a/i18n/template.xlsx
+++ b/i18n/template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" state="visible" r:id="rId3"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="1021">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -3068,6 +3068,24 @@
   </si>
   <si>
     <t xml:space="preserve">of cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Asian Avians</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds of Canada / Oiseaux du Canada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds of Continental Europe / Ngā Manu o Aotearoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds of New Zealand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Birds of U.S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">British Birds</t>
   </si>
   <si>
     <t xml:space="preserve">Value</t>
@@ -3097,19 +3115,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="12"/>
@@ -3489,7 +3504,7 @@
       <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.88"/>
@@ -10189,9 +10204,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -10199,7 +10214,7 @@
       <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.67"/>
@@ -10533,11 +10548,6 @@
       <c r="C28" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="0"/>
-      <c r="E28" s="0"/>
-      <c r="F28" s="0"/>
-      <c r="G28" s="0"/>
-      <c r="H28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -10549,11 +10559,6 @@
       <c r="C29" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="0"/>
-      <c r="E29" s="0"/>
-      <c r="F29" s="0"/>
-      <c r="G29" s="0"/>
-      <c r="H29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
@@ -10565,11 +10570,6 @@
       <c r="C30" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="0"/>
-      <c r="E30" s="0"/>
-      <c r="F30" s="0"/>
-      <c r="G30" s="0"/>
-      <c r="H30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
@@ -10581,11 +10581,6 @@
       <c r="C31" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="0"/>
-      <c r="E31" s="0"/>
-      <c r="F31" s="0"/>
-      <c r="G31" s="0"/>
-      <c r="H31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
@@ -10597,11 +10592,6 @@
       <c r="C32" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="0"/>
-      <c r="E32" s="0"/>
-      <c r="F32" s="0"/>
-      <c r="G32" s="0"/>
-      <c r="H32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
@@ -10887,31 +10877,6 @@
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0"/>
-      <c r="B54" s="0"/>
-      <c r="C54" s="0"/>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0"/>
-      <c r="B55" s="0"/>
-      <c r="C55" s="0"/>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0"/>
-      <c r="B56" s="0"/>
-      <c r="C56" s="0"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0"/>
-      <c r="B57" s="0"/>
-      <c r="C57" s="0"/>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0"/>
-      <c r="B58" s="0"/>
-      <c r="C58" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -10935,16 +10900,16 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="49.7"/>
@@ -11622,8 +11587,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;KffffffStrona &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffStrona &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -11634,15 +11599,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.56"/>
@@ -11656,35 +11621,81 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>1007</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>1008</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>1009</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>1010</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>1011</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>1012</v>
       </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -11713,7 +11724,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.95"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="11.53"/>
@@ -11724,12 +11735,12 @@
         <v>908</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>1013</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>1014</v>
+      <c r="A2" s="2" t="s">
+        <v>1020</v>
       </c>
     </row>
   </sheetData>
@@ -11738,8 +11749,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;KffffffStrona &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffStrona &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>